<commit_message>
Update Tabelas Django (treino).xlsx
</commit_message>
<xml_diff>
--- a/Módulo 03/Banco de dados/Tabelas Django (treino).xlsx
+++ b/Módulo 03/Banco de dados/Tabelas Django (treino).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALUN0-16\Documents\GitHub\Meu-Curso-Fullstack\Módulo 03\Banco de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85137864-D8B4-4571-B53D-96CC8D794C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F29024-AD56-47C8-9158-1735F8A9B19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{96686071-5522-4CCD-BC96-256FD3481093}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Tabela Usuário</t>
   </si>
@@ -108,18 +108,12 @@
     <t>sinopse</t>
   </si>
   <si>
-    <t>publicacao</t>
-  </si>
-  <si>
     <t>nacionalidade</t>
   </si>
   <si>
     <t>Tabela Categoria</t>
   </si>
   <si>
-    <t>descricao</t>
-  </si>
-  <si>
     <t>FloatField</t>
   </si>
   <si>
@@ -148,6 +142,9 @@
   </si>
   <si>
     <t>senha</t>
+  </si>
+  <si>
+    <t>data_publicacao</t>
   </si>
 </sst>
 </file>
@@ -179,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -245,11 +242,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,8 +304,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,7 +630,7 @@
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +639,7 @@
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -630,10 +659,10 @@
         <v>24</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="K3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="7"/>
+      <c r="K3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -654,10 +683,10 @@
       <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -672,7 +701,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -680,12 +709,8 @@
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -721,17 +746,17 @@
         <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -748,7 +773,7 @@
       </c>
       <c r="C10" s="9"/>
       <c r="E10" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="10"/>
       <c r="H10" s="6" t="s">
@@ -764,7 +789,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>16</v>
@@ -784,13 +809,13 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>2</v>
@@ -804,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
@@ -818,16 +843,16 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>

</xml_diff>